<commit_message>
Update Inventory Master for Feb NMPS Movies
Added February Movies
</commit_message>
<xml_diff>
--- a/Data/Bratislava NMPS Inventory - Master.xlsx
+++ b/Data/Bratislava NMPS Inventory - Master.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Red-hawk.net\Share\Data\4.Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\GitHub\NMPS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="727">
   <si>
     <t>TITLE</t>
   </si>
@@ -2157,6 +2157,54 @@
   </si>
   <si>
     <t>THE PEANUTS MOVIE</t>
+  </si>
+  <si>
+    <t>THE GOOD DINOSAUR</t>
+  </si>
+  <si>
+    <t>STAR WARS: THE FORCE AWAKENS</t>
+  </si>
+  <si>
+    <t>POINT BREAK</t>
+  </si>
+  <si>
+    <t>JEM AND THE HOLOGRAMS</t>
+  </si>
+  <si>
+    <t>CRIMSON PEAK</t>
+  </si>
+  <si>
+    <t>VICTOR FRANKENSTEIN</t>
+  </si>
+  <si>
+    <t>TRUTH</t>
+  </si>
+  <si>
+    <t>STEVE JOBS</t>
+  </si>
+  <si>
+    <t>MISS YOU ALREADY</t>
+  </si>
+  <si>
+    <t>DADDY'S HOME</t>
+  </si>
+  <si>
+    <t>SPOTLIGHT</t>
+  </si>
+  <si>
+    <t>AIRPLANE</t>
+  </si>
+  <si>
+    <t>IN THE HEART OF THE SEA</t>
+  </si>
+  <si>
+    <t>BROOKLYN</t>
+  </si>
+  <si>
+    <t>ALVIN AND THE CHIPMUNKS: THE ROAD CHIP</t>
+  </si>
+  <si>
+    <t>KRAMPUS</t>
   </si>
 </sst>
 </file>
@@ -2227,10 +2275,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C711" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:C711"/>
-  <sortState ref="A2:C711">
-    <sortCondition ref="A1:A711"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C727" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:C727"/>
+  <sortState ref="A2:C727">
+    <sortCondition ref="A1:A727"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="ID"/>
@@ -2504,10 +2552,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C711"/>
+  <dimension ref="A1:C727"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A677" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F695" sqref="F695"/>
+    <sheetView tabSelected="1" topLeftCell="A692" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A696" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A692" sqref="A692"/>
+      <selection pane="bottomLeft" activeCell="A712" sqref="A712:XFD712"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10337,6 +10387,182 @@
         <v>43770</v>
       </c>
     </row>
+    <row r="712" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A712">
+        <v>711</v>
+      </c>
+      <c r="B712" s="4" t="s">
+        <v>722</v>
+      </c>
+      <c r="C712" s="2">
+        <v>43344</v>
+      </c>
+    </row>
+    <row r="713" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A713">
+        <v>712</v>
+      </c>
+      <c r="B713" s="4" t="s">
+        <v>725</v>
+      </c>
+      <c r="C713" s="2">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="714" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A714">
+        <v>713</v>
+      </c>
+      <c r="B714" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="C714" s="2">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="715" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A715">
+        <v>714</v>
+      </c>
+      <c r="B715" s="4" t="s">
+        <v>715</v>
+      </c>
+      <c r="C715" s="2">
+        <v>43739</v>
+      </c>
+    </row>
+    <row r="716" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A716">
+        <v>715</v>
+      </c>
+      <c r="B716" s="4" t="s">
+        <v>720</v>
+      </c>
+      <c r="C716" s="2">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="717" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A717">
+        <v>716</v>
+      </c>
+      <c r="B717" s="4" t="s">
+        <v>723</v>
+      </c>
+      <c r="C717" s="2">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="718" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A718">
+        <v>717</v>
+      </c>
+      <c r="B718" s="4" t="s">
+        <v>714</v>
+      </c>
+      <c r="C718" s="2">
+        <v>43770</v>
+      </c>
+    </row>
+    <row r="719" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A719">
+        <v>718</v>
+      </c>
+      <c r="B719" s="4" t="s">
+        <v>726</v>
+      </c>
+      <c r="C719" s="2">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="720" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A720">
+        <v>719</v>
+      </c>
+      <c r="B720" s="4" t="s">
+        <v>719</v>
+      </c>
+      <c r="C720" s="2">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="721" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A721">
+        <v>720</v>
+      </c>
+      <c r="B721" s="4" t="s">
+        <v>713</v>
+      </c>
+      <c r="C721" s="2">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="722" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A722">
+        <v>721</v>
+      </c>
+      <c r="B722" s="4" t="s">
+        <v>721</v>
+      </c>
+      <c r="C722" s="2">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="723" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A723">
+        <v>722</v>
+      </c>
+      <c r="B723" s="4" t="s">
+        <v>712</v>
+      </c>
+      <c r="C723" s="2">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="724" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A724">
+        <v>723</v>
+      </c>
+      <c r="B724" s="4" t="s">
+        <v>718</v>
+      </c>
+      <c r="C724" s="2">
+        <v>43770</v>
+      </c>
+    </row>
+    <row r="725" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A725">
+        <v>724</v>
+      </c>
+      <c r="B725" s="4" t="s">
+        <v>711</v>
+      </c>
+      <c r="C725" s="2">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="726" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A726">
+        <v>725</v>
+      </c>
+      <c r="B726" s="4" t="s">
+        <v>717</v>
+      </c>
+      <c r="C726" s="2">
+        <v>43800</v>
+      </c>
+    </row>
+    <row r="727" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A727">
+        <v>726</v>
+      </c>
+      <c r="B727" s="4" t="s">
+        <v>716</v>
+      </c>
+      <c r="C727" s="2">
+        <v>43800</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>